<commit_message>
Updated CC report results. Updated GAOperators factory
</commit_message>
<xml_diff>
--- a/example/cc_reports_UKP_21.05.2018-3.8.18.985/strongly_correled_summary.xlsx
+++ b/example/cc_reports_UKP_21.05.2018-3.8.18.985/strongly_correled_summary.xlsx
@@ -473,18 +473,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -499,12 +493,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -52378,7 +52369,7 @@
   <dimension ref="A1:AW4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52399,7 +52390,7 @@
       <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">

</xml_diff>